<commit_message>
adding in extra data nad event studies
</commit_message>
<xml_diff>
--- a/Data/closure_spreadsheet_final_2019.xlsx
+++ b/Data/closure_spreadsheet_final_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924395AC-3D75-4A42-BCCB-471E3DE4831A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56623D6E-799B-5A46-94D1-C31ED0E8F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="22400" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17800" windowHeight="21900" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
   </bookViews>
   <sheets>
     <sheet name="closure_spreadsheet_main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="222">
   <si>
     <t>University</t>
   </si>
@@ -748,6 +748,12 @@
   </si>
   <si>
     <t>VA1020000</t>
+  </si>
+  <si>
+    <t>res_data_sent</t>
+  </si>
+  <si>
+    <t>res_data_received</t>
   </si>
 </sst>
 </file>
@@ -1202,11 +1208,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63494373-D1B0-2F4E-8589-31FBEC2D47DF}">
-  <dimension ref="A1:X62"/>
+  <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,7 +1222,7 @@
     <col min="21" max="21" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,8 +1295,14 @@
       <c r="X1" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1338,8 +1350,11 @@
       <c r="X2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1384,8 +1399,11 @@
       <c r="X3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1440,8 +1458,11 @@
       <c r="V4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1474,8 +1495,11 @@
       <c r="V5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1536,8 +1560,11 @@
       <c r="X6" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1576,8 +1603,11 @@
       <c r="V7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1616,8 +1646,11 @@
       <c r="V8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1651,8 +1684,11 @@
       <c r="V9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1691,8 +1727,11 @@
       <c r="V10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1731,8 +1770,11 @@
       <c r="V11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1771,8 +1813,11 @@
       <c r="V12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1817,8 +1862,11 @@
       <c r="X13" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1876,8 +1924,11 @@
       <c r="X14" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1922,8 +1973,11 @@
       <c r="X15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1962,8 +2016,11 @@
       <c r="V16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2005,8 +2062,11 @@
       <c r="X17" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2045,8 +2105,11 @@
       <c r="V18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2085,8 +2148,11 @@
       <c r="V19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2131,8 +2197,11 @@
       <c r="X20" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -2172,8 +2241,11 @@
       <c r="X21" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -2210,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2246,8 +2318,11 @@
       <c r="V23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2286,8 +2361,11 @@
       <c r="V24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -2342,8 +2420,11 @@
       <c r="V25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2377,8 +2458,11 @@
       <c r="V26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -2423,8 +2507,11 @@
       <c r="X27" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -2463,8 +2550,11 @@
       <c r="V28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2498,8 +2588,11 @@
       <c r="V29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2535,8 +2628,11 @@
       <c r="V30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2581,8 +2677,11 @@
       <c r="V31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2622,8 +2721,11 @@
       <c r="X32" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2668,8 +2770,11 @@
       <c r="X33" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -2714,8 +2819,11 @@
       <c r="X34" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -2757,8 +2865,11 @@
       <c r="X35" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -2803,8 +2914,11 @@
       <c r="X36" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -2843,8 +2957,11 @@
       <c r="V37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
@@ -2889,8 +3006,11 @@
       <c r="X38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>84</v>
       </c>
@@ -2924,8 +3044,11 @@
       <c r="V39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -2959,8 +3082,11 @@
       <c r="V40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -3005,8 +3131,11 @@
       <c r="X41" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -3061,8 +3190,11 @@
       <c r="X42" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+      <c r="Y42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -3126,8 +3258,11 @@
       <c r="X43" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>142</v>
       </c>
@@ -3135,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>143</v>
       </c>
@@ -3143,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>144</v>
       </c>
@@ -3151,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -3159,7 +3294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>146</v>
       </c>

</xml_diff>